<commit_message>
Separate each Action Cart
</commit_message>
<xml_diff>
--- a/src/test/resources/data/User_Data.xlsx
+++ b/src/test/resources/data/User_Data.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1317" uniqueCount="728">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1314" uniqueCount="725">
   <si>
     <t>1 Account dùng để test quên mật khẩu thành công</t>
   </si>
@@ -1458,18 +1458,12 @@
     <t>Tăng số lượng</t>
   </si>
   <si>
-    <t>Khi code thêm sữa hạt tươi 1 lần rồi tăng số lượng lên 5 trong giỏ hàng</t>
-  </si>
-  <si>
     <t>3,000,000</t>
   </si>
   <si>
     <t>Giảm số lượng</t>
   </si>
   <si>
-    <t>Khi code thêm 5 lần rồi giảm về 3</t>
-  </si>
-  <si>
     <t>1,000,000</t>
   </si>
   <si>
@@ -1480,9 +1474,6 @@
   </si>
   <si>
     <t>Three</t>
-  </si>
-  <si>
-    <t>Khi code thêm 1 rồi xem có giảm về 0 được không</t>
   </si>
   <si>
     <t>Product</t>
@@ -2225,7 +2216,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2263,12 +2254,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -2331,7 +2316,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="38">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2420,9 +2405,6 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -2435,16 +2417,13 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
@@ -2772,7 +2751,7 @@
         <v>28</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>714</v>
+        <v>711</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>460</v>
@@ -2798,16 +2777,16 @@
         <v>34</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>471</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>716</v>
+        <v>713</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>442</v>
@@ -2819,16 +2798,16 @@
         <v>34</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>471</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>444</v>
@@ -2836,22 +2815,22 @@
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
       <c r="A4" s="6" t="s">
-        <v>717</v>
+        <v>714</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>471</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>444</v>
@@ -2859,22 +2838,22 @@
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="6" t="s">
-        <v>718</v>
+        <v>715</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>471</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>444</v>
@@ -2882,22 +2861,22 @@
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="6" t="s">
-        <v>719</v>
+        <v>716</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>471</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>444</v>
@@ -2905,22 +2884,22 @@
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="6" t="s">
-        <v>720</v>
+        <v>717</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>471</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>444</v>
@@ -2928,22 +2907,22 @@
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="6" t="s">
-        <v>721</v>
+        <v>718</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>471</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>444</v>
@@ -2951,22 +2930,22 @@
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="6" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>471</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>444</v>
@@ -2974,22 +2953,22 @@
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="6" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>471</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>724</v>
+        <v>721</v>
       </c>
       <c r="G10" s="6" t="s">
         <v>444</v>
@@ -3001,16 +2980,16 @@
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="5" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>471</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>685</v>
+        <v>682</v>
       </c>
       <c r="G11" s="6" t="s">
         <v>444</v>
@@ -3021,19 +3000,19 @@
         <v>33</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>717</v>
+        <v>714</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>725</v>
+        <v>722</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>471</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="G12" s="6" t="s">
         <v>444</v>
@@ -3044,19 +3023,19 @@
         <v>33</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>726</v>
+        <v>723</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>725</v>
+        <v>722</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>471</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>727</v>
+        <v>724</v>
       </c>
       <c r="G13" s="6" t="s">
         <v>444</v>
@@ -10301,7 +10280,7 @@
     <col min="1" max="1" style="20" width="17.862142857142857" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="20" width="12.719285714285713" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="20" width="27.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="37" width="15.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="35" width="15.43357142857143" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="20" width="14.147857142857141" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="20" width="14.147857142857141" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="20" width="9.862142857142858" customWidth="1" bestFit="1"/>
@@ -10326,43 +10305,43 @@
         <v>27</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="33" t="s">
-        <v>611</v>
+      <c r="D1" s="32" t="s">
+        <v>608</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>29</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="G1" s="6" t="s">
+        <v>493</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>494</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>495</v>
+      </c>
+      <c r="J1" s="6" t="s">
         <v>496</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>497</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>498</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>499</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>500</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>501</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>502</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>503</v>
       </c>
       <c r="O1" s="6" t="s">
         <v>460</v>
@@ -10380,23 +10359,23 @@
         <v>440</v>
       </c>
       <c r="T1" s="6" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="U1" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="6"/>
       <c r="B2" s="6" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="33" t="s">
-        <v>614</v>
+      <c r="D2" s="32" t="s">
+        <v>611</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -10408,16 +10387,16 @@
       <c r="M2" s="6"/>
       <c r="N2" s="6"/>
       <c r="O2" s="6" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="P2" s="6" t="s">
         <v>471</v>
       </c>
-      <c r="Q2" s="38" t="s">
-        <v>565</v>
+      <c r="Q2" s="36" t="s">
+        <v>562</v>
       </c>
       <c r="R2" s="6" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="S2" s="6" t="s">
         <v>444</v>
@@ -10427,19 +10406,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="6" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="33" t="s">
-        <v>618</v>
+      <c r="D3" s="32" t="s">
+        <v>615</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
@@ -10451,16 +10430,16 @@
       <c r="M3" s="6"/>
       <c r="N3" s="6"/>
       <c r="O3" s="6" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="P3" s="6" t="s">
         <v>471</v>
       </c>
-      <c r="Q3" s="38" t="s">
-        <v>565</v>
+      <c r="Q3" s="36" t="s">
+        <v>562</v>
       </c>
       <c r="R3" s="6" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="S3" s="6" t="s">
         <v>444</v>
@@ -10470,19 +10449,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="6" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="33" t="s">
-        <v>622</v>
+      <c r="D4" s="32" t="s">
+        <v>619</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
@@ -10494,16 +10473,16 @@
       <c r="M4" s="6"/>
       <c r="N4" s="6"/>
       <c r="O4" s="6" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="P4" s="6" t="s">
         <v>471</v>
       </c>
-      <c r="Q4" s="38" t="s">
-        <v>565</v>
+      <c r="Q4" s="36" t="s">
+        <v>562</v>
       </c>
       <c r="R4" s="6" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="S4" s="6" t="s">
         <v>444</v>
@@ -10513,19 +10492,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="6" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="33" t="s">
-        <v>626</v>
+      <c r="D5" s="32" t="s">
+        <v>623</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
@@ -10537,16 +10516,16 @@
       <c r="M5" s="6"/>
       <c r="N5" s="6"/>
       <c r="O5" s="6" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="P5" s="6" t="s">
         <v>471</v>
       </c>
-      <c r="Q5" s="38" t="s">
-        <v>565</v>
+      <c r="Q5" s="36" t="s">
+        <v>562</v>
       </c>
       <c r="R5" s="6" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="S5" s="6" t="s">
         <v>444</v>
@@ -10556,17 +10535,17 @@
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="6" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="33" t="s">
-        <v>629</v>
+      <c r="D6" s="32" t="s">
+        <v>626</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
@@ -10578,16 +10557,16 @@
       <c r="M6" s="6"/>
       <c r="N6" s="6"/>
       <c r="O6" s="6" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="P6" s="6" t="s">
         <v>471</v>
       </c>
-      <c r="Q6" s="38" t="s">
-        <v>565</v>
+      <c r="Q6" s="36" t="s">
+        <v>562</v>
       </c>
       <c r="R6" s="5" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="S6" s="6" t="s">
         <v>444</v>
@@ -10597,19 +10576,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="6" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="33" t="s">
-        <v>632</v>
+      <c r="D7" s="32" t="s">
+        <v>629</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
@@ -10621,16 +10600,16 @@
       <c r="M7" s="6"/>
       <c r="N7" s="6"/>
       <c r="O7" s="6" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="P7" s="6" t="s">
         <v>471</v>
       </c>
-      <c r="Q7" s="38" t="s">
-        <v>565</v>
+      <c r="Q7" s="36" t="s">
+        <v>562</v>
       </c>
       <c r="R7" s="6" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="S7" s="6" t="s">
         <v>444</v>
@@ -10640,19 +10619,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="6" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="33" t="s">
-        <v>635</v>
+      <c r="D8" s="32" t="s">
+        <v>632</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
@@ -10664,16 +10643,16 @@
       <c r="M8" s="6"/>
       <c r="N8" s="6"/>
       <c r="O8" s="6" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="P8" s="6" t="s">
         <v>471</v>
       </c>
-      <c r="Q8" s="38" t="s">
-        <v>565</v>
+      <c r="Q8" s="36" t="s">
+        <v>562</v>
       </c>
       <c r="R8" s="6" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="S8" s="6" t="s">
         <v>444</v>
@@ -10683,19 +10662,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="6" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="33" t="s">
-        <v>635</v>
+      <c r="D9" s="32" t="s">
+        <v>632</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
@@ -10707,16 +10686,16 @@
       <c r="M9" s="6"/>
       <c r="N9" s="6"/>
       <c r="O9" s="6" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="P9" s="6" t="s">
         <v>471</v>
       </c>
-      <c r="Q9" s="38" t="s">
-        <v>565</v>
+      <c r="Q9" s="36" t="s">
+        <v>562</v>
       </c>
       <c r="R9" s="6" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="S9" s="6" t="s">
         <v>444</v>
@@ -10726,19 +10705,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="6" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="33" t="s">
-        <v>640</v>
+      <c r="D10" s="32" t="s">
+        <v>637</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
@@ -10750,16 +10729,16 @@
       <c r="M10" s="6"/>
       <c r="N10" s="6"/>
       <c r="O10" s="6" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="P10" s="6" t="s">
         <v>471</v>
       </c>
-      <c r="Q10" s="38" t="s">
-        <v>565</v>
+      <c r="Q10" s="36" t="s">
+        <v>562</v>
       </c>
       <c r="R10" s="6" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="S10" s="6" t="s">
         <v>444</v>
@@ -10769,19 +10748,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="6" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="33" t="s">
-        <v>643</v>
+      <c r="D11" s="32" t="s">
+        <v>640</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
@@ -10793,16 +10772,16 @@
       <c r="M11" s="6"/>
       <c r="N11" s="6"/>
       <c r="O11" s="6" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="P11" s="6" t="s">
         <v>471</v>
       </c>
-      <c r="Q11" s="38" t="s">
-        <v>565</v>
+      <c r="Q11" s="36" t="s">
+        <v>562</v>
       </c>
       <c r="R11" s="6" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="S11" s="6" t="s">
         <v>444</v>
@@ -10812,17 +10791,17 @@
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="6" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="39"/>
+      <c r="D12" s="37"/>
       <c r="E12" s="6" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
@@ -10834,16 +10813,16 @@
       <c r="M12" s="6"/>
       <c r="N12" s="6"/>
       <c r="O12" s="6" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="P12" s="6" t="s">
         <v>471</v>
       </c>
-      <c r="Q12" s="38" t="s">
-        <v>565</v>
+      <c r="Q12" s="36" t="s">
+        <v>562</v>
       </c>
       <c r="R12" s="5" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="S12" s="6" t="s">
         <v>444</v>
@@ -10853,19 +10832,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="6" t="s">
+        <v>642</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>645</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>648</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="33" t="s">
-        <v>514</v>
+      <c r="D13" s="32" t="s">
+        <v>511</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
@@ -10877,16 +10856,16 @@
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
       <c r="O13" s="6" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="P13" s="6" t="s">
         <v>471</v>
       </c>
-      <c r="Q13" s="38" t="s">
-        <v>565</v>
+      <c r="Q13" s="36" t="s">
+        <v>562</v>
       </c>
       <c r="R13" s="6" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="S13" s="6" t="s">
         <v>444</v>
@@ -10896,19 +10875,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="6" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="33" t="s">
-        <v>651</v>
+      <c r="D14" s="32" t="s">
+        <v>648</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
@@ -10920,16 +10899,16 @@
       <c r="M14" s="6"/>
       <c r="N14" s="6"/>
       <c r="O14" s="6" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="P14" s="6" t="s">
         <v>471</v>
       </c>
-      <c r="Q14" s="38" t="s">
-        <v>565</v>
+      <c r="Q14" s="36" t="s">
+        <v>562</v>
       </c>
       <c r="R14" s="6" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="S14" s="6" t="s">
         <v>444</v>
@@ -10939,19 +10918,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="6" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="33" t="s">
-        <v>654</v>
+      <c r="D15" s="32" t="s">
+        <v>651</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
@@ -10963,16 +10942,16 @@
       <c r="M15" s="6"/>
       <c r="N15" s="6"/>
       <c r="O15" s="6" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="P15" s="6" t="s">
         <v>471</v>
       </c>
-      <c r="Q15" s="38" t="s">
-        <v>565</v>
+      <c r="Q15" s="36" t="s">
+        <v>562</v>
       </c>
       <c r="R15" s="6" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
       <c r="S15" s="6" t="s">
         <v>444</v>
@@ -10982,19 +10961,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="6" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="33" t="s">
-        <v>657</v>
+      <c r="D16" s="32" t="s">
+        <v>654</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
@@ -11006,16 +10985,16 @@
       <c r="M16" s="6"/>
       <c r="N16" s="6"/>
       <c r="O16" s="6" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="P16" s="6" t="s">
         <v>471</v>
       </c>
-      <c r="Q16" s="38" t="s">
-        <v>565</v>
+      <c r="Q16" s="36" t="s">
+        <v>562</v>
       </c>
       <c r="R16" s="6" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="S16" s="6" t="s">
         <v>444</v>
@@ -11025,17 +11004,17 @@
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="6" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="C17" s="6"/>
-      <c r="D17" s="33" t="s">
-        <v>661</v>
+      <c r="D17" s="32" t="s">
+        <v>658</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
@@ -11047,16 +11026,16 @@
       <c r="M17" s="6"/>
       <c r="N17" s="6"/>
       <c r="O17" s="6" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="P17" s="6" t="s">
         <v>471</v>
       </c>
-      <c r="Q17" s="38" t="s">
-        <v>565</v>
+      <c r="Q17" s="36" t="s">
+        <v>562</v>
       </c>
       <c r="R17" s="6" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="S17" s="6" t="s">
         <v>444</v>
@@ -11066,19 +11045,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="6" t="s">
+        <v>656</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>659</v>
       </c>
-      <c r="B18" s="6" t="s">
-        <v>662</v>
-      </c>
       <c r="C18" s="6" t="s">
-        <v>514</v>
-      </c>
-      <c r="D18" s="33" t="s">
-        <v>663</v>
+        <v>511</v>
+      </c>
+      <c r="D18" s="32" t="s">
+        <v>660</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
@@ -11090,16 +11069,16 @@
       <c r="M18" s="6"/>
       <c r="N18" s="6"/>
       <c r="O18" s="6" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="P18" s="6" t="s">
         <v>471</v>
       </c>
-      <c r="Q18" s="38" t="s">
-        <v>565</v>
+      <c r="Q18" s="36" t="s">
+        <v>562</v>
       </c>
       <c r="R18" s="6" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="S18" s="6" t="s">
         <v>444</v>
@@ -11109,19 +11088,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="6" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>666</v>
-      </c>
-      <c r="D19" s="33" t="s">
-        <v>667</v>
+        <v>663</v>
+      </c>
+      <c r="D19" s="32" t="s">
+        <v>664</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
@@ -11133,16 +11112,16 @@
       <c r="M19" s="6"/>
       <c r="N19" s="6"/>
       <c r="O19" s="6" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="P19" s="6" t="s">
         <v>471</v>
       </c>
-      <c r="Q19" s="38" t="s">
-        <v>565</v>
+      <c r="Q19" s="36" t="s">
+        <v>562</v>
       </c>
       <c r="R19" s="6" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="S19" s="6" t="s">
         <v>444</v>
@@ -11152,19 +11131,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="6" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>669</v>
-      </c>
-      <c r="D20" s="33" t="s">
-        <v>670</v>
+        <v>666</v>
+      </c>
+      <c r="D20" s="32" t="s">
+        <v>667</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
@@ -11176,16 +11155,16 @@
       <c r="M20" s="6"/>
       <c r="N20" s="6"/>
       <c r="O20" s="6" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
       <c r="P20" s="6" t="s">
         <v>471</v>
       </c>
-      <c r="Q20" s="38" t="s">
-        <v>565</v>
+      <c r="Q20" s="36" t="s">
+        <v>562</v>
       </c>
       <c r="R20" s="6" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="S20" s="6" t="s">
         <v>444</v>
@@ -11195,19 +11174,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="6" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>673</v>
-      </c>
-      <c r="D21" s="33" t="s">
-        <v>674</v>
+        <v>670</v>
+      </c>
+      <c r="D21" s="32" t="s">
+        <v>671</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
@@ -11219,16 +11198,16 @@
       <c r="M21" s="6"/>
       <c r="N21" s="6"/>
       <c r="O21" s="6" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="P21" s="6" t="s">
         <v>471</v>
       </c>
-      <c r="Q21" s="38" t="s">
-        <v>565</v>
+      <c r="Q21" s="36" t="s">
+        <v>562</v>
       </c>
       <c r="R21" s="6" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="S21" s="6" t="s">
         <v>444</v>
@@ -11238,19 +11217,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="6" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>676</v>
-      </c>
-      <c r="D22" s="33" t="s">
-        <v>677</v>
+        <v>673</v>
+      </c>
+      <c r="D22" s="32" t="s">
+        <v>674</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
@@ -11262,16 +11241,16 @@
       <c r="M22" s="6"/>
       <c r="N22" s="6"/>
       <c r="O22" s="6" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
       <c r="P22" s="6" t="s">
         <v>471</v>
       </c>
-      <c r="Q22" s="38" t="s">
-        <v>565</v>
+      <c r="Q22" s="36" t="s">
+        <v>562</v>
       </c>
       <c r="R22" s="6" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="S22" s="6" t="s">
         <v>444</v>
@@ -11281,19 +11260,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="6" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>547</v>
-      </c>
-      <c r="D23" s="33" t="s">
-        <v>680</v>
+        <v>544</v>
+      </c>
+      <c r="D23" s="32" t="s">
+        <v>677</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
@@ -11305,16 +11284,16 @@
       <c r="M23" s="6"/>
       <c r="N23" s="6"/>
       <c r="O23" s="6" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
       <c r="P23" s="6" t="s">
         <v>471</v>
       </c>
-      <c r="Q23" s="38" t="s">
-        <v>565</v>
+      <c r="Q23" s="36" t="s">
+        <v>562</v>
       </c>
       <c r="R23" s="6" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="S23" s="6" t="s">
         <v>444</v>
@@ -11324,16 +11303,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="6" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D24" s="33" t="s">
-        <v>683</v>
+      <c r="D24" s="32" t="s">
+        <v>680</v>
       </c>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
@@ -11346,16 +11325,16 @@
       <c r="M24" s="6"/>
       <c r="N24" s="6"/>
       <c r="O24" s="6" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
       <c r="P24" s="6" t="s">
         <v>471</v>
       </c>
-      <c r="Q24" s="38" t="s">
-        <v>565</v>
+      <c r="Q24" s="36" t="s">
+        <v>562</v>
       </c>
       <c r="R24" s="6" t="s">
-        <v>685</v>
+        <v>682</v>
       </c>
       <c r="S24" s="6" t="s">
         <v>444</v>
@@ -11365,19 +11344,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="6" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D25" s="33" t="s">
-        <v>688</v>
+      <c r="D25" s="32" t="s">
+        <v>685</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
@@ -11389,16 +11368,16 @@
       <c r="M25" s="6"/>
       <c r="N25" s="6"/>
       <c r="O25" s="6" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="P25" s="6" t="s">
         <v>471</v>
       </c>
-      <c r="Q25" s="38" t="s">
-        <v>565</v>
+      <c r="Q25" s="36" t="s">
+        <v>562</v>
       </c>
       <c r="R25" s="6" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="S25" s="6" t="s">
         <v>444</v>
@@ -11408,22 +11387,22 @@
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="6" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D26" s="33" t="s">
-        <v>692</v>
+      <c r="D26" s="32" t="s">
+        <v>689</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
@@ -11434,16 +11413,16 @@
       <c r="M26" s="6"/>
       <c r="N26" s="6"/>
       <c r="O26" s="6" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="P26" s="6" t="s">
         <v>471</v>
       </c>
-      <c r="Q26" s="38" t="s">
-        <v>565</v>
+      <c r="Q26" s="36" t="s">
+        <v>562</v>
       </c>
       <c r="R26" s="6" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
       <c r="S26" s="6" t="s">
         <v>444</v>
@@ -11453,19 +11432,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
       <c r="A27" s="6" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D27" s="33" t="s">
-        <v>697</v>
+      <c r="D27" s="32" t="s">
+        <v>694</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
@@ -11477,85 +11456,85 @@
       <c r="M27" s="6"/>
       <c r="N27" s="6"/>
       <c r="O27" s="6" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
       <c r="P27" s="6" t="s">
         <v>471</v>
       </c>
-      <c r="Q27" s="38" t="s">
-        <v>565</v>
+      <c r="Q27" s="36" t="s">
+        <v>562</v>
       </c>
       <c r="R27" s="6" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
       <c r="S27" s="6" t="s">
         <v>442</v>
       </c>
       <c r="T27" s="6" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
       <c r="U27" s="24"/>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
       <c r="A28" s="6" t="s">
-        <v>701</v>
+        <v>698</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D28" s="33" t="s">
+      <c r="D28" s="32" t="s">
+        <v>700</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>612</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>701</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>517</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>702</v>
+      </c>
+      <c r="I28" s="6" t="s">
         <v>703</v>
       </c>
-      <c r="E28" s="6" t="s">
-        <v>615</v>
-      </c>
-      <c r="F28" s="6" t="s">
+      <c r="J28" s="6" t="s">
         <v>704</v>
       </c>
-      <c r="G28" s="6" t="s">
-        <v>520</v>
-      </c>
-      <c r="H28" s="6" t="s">
+      <c r="K28" s="6" t="s">
         <v>705</v>
       </c>
-      <c r="I28" s="6" t="s">
+      <c r="L28" s="6" t="s">
         <v>706</v>
       </c>
-      <c r="J28" s="6" t="s">
+      <c r="M28" s="6" t="s">
         <v>707</v>
       </c>
-      <c r="K28" s="6" t="s">
+      <c r="N28" s="6" t="s">
         <v>708</v>
       </c>
-      <c r="L28" s="6" t="s">
-        <v>709</v>
-      </c>
-      <c r="M28" s="6" t="s">
-        <v>710</v>
-      </c>
-      <c r="N28" s="6" t="s">
-        <v>711</v>
-      </c>
       <c r="O28" s="6" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
       <c r="P28" s="6" t="s">
         <v>471</v>
       </c>
-      <c r="Q28" s="38" t="s">
-        <v>565</v>
+      <c r="Q28" s="36" t="s">
+        <v>562</v>
       </c>
       <c r="R28" s="6" t="s">
-        <v>712</v>
+        <v>709</v>
       </c>
       <c r="S28" s="6" t="s">
         <v>442</v>
       </c>
       <c r="T28" s="6" t="s">
-        <v>713</v>
+        <v>710</v>
       </c>
       <c r="U28" s="24"/>
     </row>
@@ -11575,7 +11554,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="37" width="16.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="35" width="16.433571428571426" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="20" width="18.14785714285714" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="20" width="7.433571428571429" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="20" width="84.57642857142856" customWidth="1" bestFit="1"/>
@@ -11599,13 +11578,13 @@
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
-      <c r="A1" s="33" t="s">
-        <v>587</v>
+      <c r="A1" s="32" t="s">
+        <v>584</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>460</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="36" t="s">
         <v>461</v>
       </c>
       <c r="D1" s="6" t="s">
@@ -11619,68 +11598,68 @@
       </c>
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
-      <c r="I1" s="38"/>
+      <c r="I1" s="36"/>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
       <c r="L1" s="6"/>
       <c r="M1" s="6"/>
-      <c r="N1" s="38"/>
+      <c r="N1" s="36"/>
       <c r="O1" s="6"/>
       <c r="P1" s="6"/>
       <c r="Q1" s="6"/>
       <c r="R1" s="6"/>
-      <c r="S1" s="38"/>
+      <c r="S1" s="36"/>
       <c r="T1" s="6"/>
       <c r="U1" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="33" t="s">
-        <v>486</v>
+      <c r="A2" s="32" t="s">
+        <v>483</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>471</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>442</v>
       </c>
       <c r="G2" s="6"/>
-      <c r="H2" s="38"/>
+      <c r="H2" s="36"/>
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
-      <c r="M2" s="38"/>
+      <c r="M2" s="36"/>
       <c r="N2" s="6"/>
       <c r="O2" s="6"/>
       <c r="P2" s="6"/>
       <c r="Q2" s="6"/>
-      <c r="R2" s="38"/>
+      <c r="R2" s="36"/>
       <c r="S2" s="6"/>
       <c r="T2" s="6"/>
       <c r="U2" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="33"/>
+      <c r="A3" s="32"/>
       <c r="B3" s="6" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>471</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>442</v>
@@ -11702,20 +11681,20 @@
       <c r="U3" s="24"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="33" t="s">
-        <v>514</v>
+      <c r="A4" s="32" t="s">
+        <v>511</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>471</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>442</v>
@@ -11737,20 +11716,20 @@
       <c r="U4" s="24"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="33" t="s">
-        <v>595</v>
+      <c r="A5" s="32" t="s">
+        <v>592</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>471</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>444</v>
@@ -11772,20 +11751,20 @@
       <c r="U5" s="24"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="33" t="s">
-        <v>599</v>
+      <c r="A6" s="32" t="s">
+        <v>596</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>471</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>442</v>
@@ -11807,20 +11786,20 @@
       <c r="U6" s="24"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="33" t="s">
-        <v>602</v>
+      <c r="A7" s="32" t="s">
+        <v>599</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>471</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>442</v>
@@ -11842,20 +11821,20 @@
       <c r="U7" s="24"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
-      <c r="A8" s="33">
+      <c r="A8" s="32">
         <v>1000000</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>471</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>444</v>
@@ -11877,20 +11856,20 @@
       <c r="U8" s="24"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
-      <c r="A9" s="33" t="s">
-        <v>607</v>
+      <c r="A9" s="32" t="s">
+        <v>604</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>471</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>444</v>
@@ -11928,7 +11907,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="20" width="27.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="37" width="12.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="35" width="12.719285714285713" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="20" width="12.719285714285713" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="20" width="44.43357142857143" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="20" width="9.147857142857141" customWidth="1" bestFit="1"/>
@@ -11942,11 +11921,11 @@
       <c r="A1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="33" t="s">
-        <v>567</v>
+      <c r="B1" s="32" t="s">
+        <v>564</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>460</v>
@@ -11969,21 +11948,21 @@
       <c r="A2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="33"/>
+      <c r="B2" s="32"/>
       <c r="C2" s="6" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>471</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>444</v>
@@ -11994,23 +11973,23 @@
       <c r="A3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="33">
+      <c r="B3" s="32">
         <v>123</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>471</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>444</v>
@@ -12021,23 +12000,23 @@
       <c r="A4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="33" t="s">
-        <v>514</v>
+      <c r="B4" s="32" t="s">
+        <v>511</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>471</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="H4" s="6" t="s">
         <v>444</v>
@@ -12048,23 +12027,23 @@
       <c r="A5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="32" t="s">
         <v>34</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>471</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="H5" s="6" t="s">
         <v>444</v>
@@ -12075,21 +12054,21 @@
       <c r="A6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="32" t="s">
         <v>34</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="5" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>471</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="H6" s="6" t="s">
         <v>444</v>
@@ -12100,23 +12079,23 @@
       <c r="A7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="32" t="s">
         <v>34</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>471</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="H7" s="6" t="s">
         <v>444</v>
@@ -12127,23 +12106,23 @@
       <c r="A8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="32" t="s">
         <v>34</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>471</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="H8" s="6" t="s">
         <v>442</v>
@@ -12182,10 +12161,10 @@
         <v>28</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>460</v>
@@ -12203,28 +12182,28 @@
         <v>440</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="6"/>
       <c r="B2" s="6" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>471</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>444</v>
@@ -12233,25 +12212,25 @@
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="6" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>471</v>
       </c>
       <c r="F3" s="6" t="s">
+        <v>532</v>
+      </c>
+      <c r="G3" s="6" t="s">
         <v>535</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>538</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>444</v>
@@ -12260,25 +12239,25 @@
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="6" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>471</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="H4" s="6" t="s">
         <v>444</v>
@@ -12287,25 +12266,25 @@
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="6" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>471</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="H5" s="6" t="s">
         <v>444</v>
@@ -12314,25 +12293,25 @@
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="6" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>471</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="H6" s="6" t="s">
         <v>444</v>
@@ -12341,25 +12320,25 @@
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="6" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>471</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="H7" s="6" t="s">
         <v>444</v>
@@ -12368,25 +12347,25 @@
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="6" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>471</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="H8" s="6" t="s">
         <v>444</v>
@@ -12397,21 +12376,21 @@
       <c r="A9" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="33"/>
+      <c r="B9" s="32"/>
       <c r="C9" s="6" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>471</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="H9" s="6" t="s">
         <v>444</v>
@@ -12422,23 +12401,23 @@
       <c r="A10" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="33" t="s">
-        <v>514</v>
+      <c r="B10" s="32" t="s">
+        <v>511</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>471</v>
       </c>
       <c r="F10" s="6" t="s">
+        <v>547</v>
+      </c>
+      <c r="G10" s="6" t="s">
         <v>550</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>553</v>
       </c>
       <c r="H10" s="6" t="s">
         <v>444</v>
@@ -12450,22 +12429,22 @@
         <v>1</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>471</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="H11" s="6" t="s">
         <v>444</v>
@@ -12477,20 +12456,20 @@
         <v>1</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>532</v>
-      </c>
-      <c r="C12" s="33"/>
+        <v>529</v>
+      </c>
+      <c r="C12" s="32"/>
       <c r="D12" s="5" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>471</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="H12" s="6" t="s">
         <v>444</v>
@@ -12502,22 +12481,22 @@
         <v>1</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>471</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="H13" s="6" t="s">
         <v>444</v>
@@ -12529,28 +12508,28 @@
         <v>1</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>471</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="H14" s="6" t="s">
         <v>444</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
@@ -12558,28 +12537,28 @@
         <v>1</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>471</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="H15" s="6" t="s">
         <v>444</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
@@ -12587,28 +12566,28 @@
         <v>1</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>471</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="H16" s="6" t="s">
         <v>442</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
     </row>
   </sheetData>
@@ -12649,31 +12628,31 @@
         <v>27</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>492</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>493</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>494</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>495</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>496</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>497</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>498</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>499</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>500</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>501</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>502</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>503</v>
       </c>
       <c r="K1" s="6" t="s">
         <v>460</v>
@@ -12694,7 +12673,7 @@
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="6"/>
       <c r="B2" s="6" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
@@ -12705,16 +12684,16 @@
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
       <c r="K2" s="6" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="L2" s="6" t="s">
         <v>471</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="O2" s="6" t="s">
         <v>444</v>
@@ -12722,10 +12701,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="6" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
@@ -12736,16 +12715,16 @@
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
       <c r="K3" s="6" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="L3" s="6" t="s">
         <v>471</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="O3" s="6" t="s">
         <v>444</v>
@@ -12753,7 +12732,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="6" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -12765,16 +12744,16 @@
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
       <c r="K4" s="6" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="L4" s="6" t="s">
         <v>471</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="O4" s="6" t="s">
         <v>444</v>
@@ -12782,10 +12761,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="6" t="s">
+        <v>508</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>511</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>514</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
@@ -12796,16 +12775,16 @@
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
       <c r="K5" s="6" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="L5" s="6" t="s">
         <v>471</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="O5" s="6" t="s">
         <v>444</v>
@@ -12813,10 +12792,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="6" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
@@ -12827,16 +12806,16 @@
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
       <c r="K6" s="6" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="L6" s="6" t="s">
         <v>471</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="O6" s="6" t="s">
         <v>442</v>
@@ -12844,46 +12823,46 @@
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="6" t="s">
+        <v>514</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>501</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>517</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>504</v>
-      </c>
-      <c r="C7" s="6" t="s">
+      <c r="D7" s="6" t="s">
+        <v>518</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>519</v>
+      </c>
+      <c r="F7" s="6" t="s">
         <v>520</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="G7" s="6" t="s">
         <v>521</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="H7" s="6" t="s">
         <v>522</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="I7" s="6" t="s">
         <v>523</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="J7" s="6" t="s">
         <v>524</v>
       </c>
-      <c r="H7" s="6" t="s">
-        <v>525</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>526</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>527</v>
-      </c>
       <c r="K7" s="6" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="L7" s="6" t="s">
         <v>471</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="O7" s="6" t="s">
         <v>442</v>
@@ -12935,7 +12914,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="6" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>471</v>
@@ -12944,7 +12923,7 @@
         <v>472</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>444</v>
@@ -12955,7 +12934,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="6" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>471</v>
@@ -12964,7 +12943,7 @@
         <v>472</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>444</v>
@@ -12975,22 +12954,22 @@
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="6" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>471</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>442</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
   </sheetData>
@@ -13010,7 +12989,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="20" width="13.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="36" width="9.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="34" width="9.147857142857141" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="20" width="10.576428571428572" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="20" width="31.433571428571426" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="20" width="8.43357142857143" customWidth="1" bestFit="1"/>
@@ -13022,9 +13001,9 @@
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="6" t="s">
-        <v>483</v>
-      </c>
-      <c r="B1" s="33" t="s">
+        <v>480</v>
+      </c>
+      <c r="B1" s="32" t="s">
         <v>468</v>
       </c>
       <c r="C1" s="6" t="s">
@@ -13051,13 +13030,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="6" t="s">
-        <v>479</v>
-      </c>
-      <c r="B2" s="34">
+        <v>477</v>
+      </c>
+      <c r="B2" s="33">
         <v>1</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>470</v>
@@ -13069,7 +13048,7 @@
         <v>472</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>29</v>
@@ -13078,13 +13057,13 @@
         <v>465</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="35"/>
-      <c r="B3" s="34">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
+      <c r="A3" s="7"/>
+      <c r="B3" s="33">
         <v>3</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>470</v>
@@ -13096,7 +13075,7 @@
         <v>472</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>29</v>
@@ -13107,9 +13086,9 @@
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="6" t="s">
-        <v>486</v>
-      </c>
-      <c r="B4" s="34">
+        <v>483</v>
+      </c>
+      <c r="B4" s="33">
         <v>5</v>
       </c>
       <c r="C4" s="6" t="s">
@@ -13125,13 +13104,13 @@
         <v>472</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="H4" s="6" t="s">
         <v>29</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
   </sheetData>
@@ -13144,21 +13123,20 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="32" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="31" width="14.147857142857141" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="20" width="10.576428571428572" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="20" width="12.576428571428572" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="20" width="9.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="20" width="21.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="20" width="29.14785714285714" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="20" width="35.43357142857143" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="20" width="9.005" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="20" width="9.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="20" width="61.71928571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
@@ -13186,10 +13164,9 @@
       <c r="H1" s="6" t="s">
         <v>463</v>
       </c>
-      <c r="I1" s="7"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
-      <c r="A2" s="31">
+      <c r="A2" s="30">
         <v>5</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -13213,16 +13190,13 @@
       <c r="H2" s="6" t="s">
         <v>465</v>
       </c>
-      <c r="I2" s="6" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
+      <c r="A3" s="30">
+        <v>3</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>474</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
-      <c r="A3" s="31">
-        <v>3</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>475</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>470</v>
@@ -13234,7 +13208,7 @@
         <v>472</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>29</v>
@@ -13242,19 +13216,16 @@
       <c r="H3" s="6" t="s">
         <v>467</v>
       </c>
-      <c r="I3" s="6" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.25">
+      <c r="A4" s="30">
+        <v>1</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>476</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>477</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.25">
-      <c r="A4" s="31">
-        <v>1</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>478</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>479</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>471</v>
@@ -13263,16 +13234,13 @@
         <v>472</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>444</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>481</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add file data and edit file test login, changePass
</commit_message>
<xml_diff>
--- a/src/test/resources/data/User_Data.xlsx
+++ b/src/test/resources/data/User_Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="9"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Login"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1319" uniqueCount="726">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1327" uniqueCount="726">
   <si>
     <t>1 Account dùng để test quên mật khẩu thành công</t>
   </si>
@@ -2800,7 +2800,7 @@
         <v>444</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="6" t="s">
         <v>715</v>
       </c>
@@ -2982,7 +2982,7 @@
         <v>444</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="33">
       <c r="A12" s="6" t="s">
         <v>33</v>
       </c>
@@ -3005,7 +3005,7 @@
         <v>444</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="33">
       <c r="A13" s="6" t="s">
         <v>33</v>
       </c>
@@ -3040,7 +3040,7 @@
   </sheetPr>
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -11565,234 +11565,259 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="20" width="27.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="30" width="12.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="20" width="12.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="20" width="44.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="20" width="9.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="20" width="33.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="20" width="29.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="20" width="9.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="25" width="13.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="25" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="30" width="16.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="20" width="12.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="20" width="44.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="20" width="9.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="20" width="33.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="20" width="29.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="20" width="9.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="25" width="13.719285714285713" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="29" t="s">
         <v>565</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>566</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>459</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>460</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>461</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>439</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>440</v>
       </c>
-      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="6" t="s">
+      <c r="B2" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="29"/>
+      <c r="D2" s="6" t="s">
         <v>567</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>568</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>464</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>569</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>570</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>444</v>
       </c>
-      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="29">
+      <c r="B3" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="29">
         <v>123</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="D3" s="6" t="s">
         <v>571</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="E3" s="6" t="s">
         <v>572</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="6" t="s">
         <v>464</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="G3" s="6" t="s">
         <v>569</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="H3" s="6" t="s">
         <v>573</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="I3" s="6" t="s">
         <v>444</v>
       </c>
-      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="29" t="s">
         <v>512</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="D4" s="6" t="s">
         <v>574</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="E4" s="6" t="s">
         <v>575</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="F4" s="6" t="s">
         <v>464</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="G4" s="6" t="s">
         <v>569</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="H4" s="6" t="s">
         <v>576</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="I4" s="6" t="s">
         <v>444</v>
       </c>
-      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>577</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="F5" s="6" t="s">
         <v>464</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="G5" s="6" t="s">
         <v>569</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="H5" s="6" t="s">
         <v>578</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="I5" s="6" t="s">
         <v>444</v>
       </c>
-      <c r="I5" s="24"/>
+      <c r="J5" s="24"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="5" t="s">
+      <c r="C6" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="5" t="s">
         <v>547</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="F6" s="6" t="s">
         <v>464</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="G6" s="6" t="s">
         <v>569</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="H6" s="6" t="s">
         <v>579</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="I6" s="6" t="s">
         <v>444</v>
       </c>
-      <c r="I6" s="24"/>
+      <c r="J6" s="24"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>580</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="E7" s="6" t="s">
         <v>575</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="F7" s="6" t="s">
         <v>464</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="G7" s="6" t="s">
         <v>569</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="H7" s="6" t="s">
         <v>581</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="I7" s="6" t="s">
         <v>444</v>
       </c>
-      <c r="I7" s="24"/>
+      <c r="J7" s="24"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>567</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="E8" s="6" t="s">
         <v>582</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="F8" s="6" t="s">
         <v>464</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="G8" s="6" t="s">
         <v>583</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="H8" s="6" t="s">
         <v>584</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="I8" s="6" t="s">
         <v>442</v>
       </c>
-      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Done Creat data and Update Test
</commit_message>
<xml_diff>
--- a/src/test/resources/data/User_Data.xlsx
+++ b/src/test/resources/data/User_Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Login"/>
@@ -13,10 +13,10 @@
     <sheet r:id="rId4" sheetId="4" name="ChangePass"/>
     <sheet r:id="rId5" sheetId="5" name="ForgotPass"/>
     <sheet r:id="rId6" sheetId="6" name="Information"/>
-    <sheet r:id="rId7" sheetId="7" name="SCart"/>
-    <sheet r:id="rId8" sheetId="8" name="SCartAdd"/>
-    <sheet r:id="rId9" sheetId="9" name="SCartUpd"/>
-    <sheet r:id="rId10" sheetId="10" name="SCartDel"/>
+    <sheet r:id="rId7" sheetId="7" name="Cart"/>
+    <sheet r:id="rId8" sheetId="8" name="CartAdd"/>
+    <sheet r:id="rId9" sheetId="9" name="CartUpdate"/>
+    <sheet r:id="rId10" sheetId="10" name="CartDelete"/>
     <sheet r:id="rId11" sheetId="11" name="Order_Bank"/>
     <sheet r:id="rId12" sheetId="12" name="Order_Indrect"/>
     <sheet r:id="rId13" sheetId="13" name="Order_Direct"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1327" uniqueCount="726">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1328" uniqueCount="727">
   <si>
     <t>1 Account dùng để test quên mật khẩu thành công</t>
   </si>
@@ -1483,6 +1483,9 @@
   </si>
   <si>
     <t>Thêm 1 sản phẩm vào giỏ hàng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   </t>
   </si>
   <si>
     <t>Thêm nhiều sản phẩm vào giỏ hàng</t>
@@ -2738,7 +2741,7 @@
         <v>28</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>459</v>
@@ -2764,16 +2767,16 @@
         <v>34</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>464</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>442</v>
@@ -2785,16 +2788,16 @@
         <v>34</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>464</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>444</v>
@@ -2802,22 +2805,22 @@
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="6" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>464</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>444</v>
@@ -2825,22 +2828,22 @@
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="6" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>464</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>444</v>
@@ -2848,22 +2851,22 @@
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="6" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>464</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>444</v>
@@ -2871,22 +2874,22 @@
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="6" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>464</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>444</v>
@@ -2894,22 +2897,22 @@
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="6" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>464</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>444</v>
@@ -2917,22 +2920,22 @@
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="6" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>464</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>444</v>
@@ -2940,22 +2943,22 @@
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="6" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>464</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="G10" s="6" t="s">
         <v>444</v>
@@ -2967,16 +2970,16 @@
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="5" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>464</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="G11" s="6" t="s">
         <v>444</v>
@@ -2987,19 +2990,19 @@
         <v>33</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>464</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="G12" s="6" t="s">
         <v>444</v>
@@ -3010,19 +3013,19 @@
         <v>33</v>
       </c>
       <c r="B13" s="6" t="s">
+        <v>725</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>724</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>723</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>464</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="G13" s="6" t="s">
         <v>444</v>
@@ -3040,7 +3043,7 @@
   </sheetPr>
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -9970,43 +9973,43 @@
         <v>27</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>28</v>
       </c>
       <c r="D1" s="29" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>29</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="O1" s="6" t="s">
         <v>459</v>
@@ -10024,23 +10027,23 @@
         <v>440</v>
       </c>
       <c r="T1" s="6" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="U1" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="6"/>
       <c r="B2" s="6" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>13</v>
       </c>
       <c r="D2" s="29" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
@@ -10052,16 +10055,16 @@
       <c r="M2" s="6"/>
       <c r="N2" s="6"/>
       <c r="O2" s="6" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="P2" s="6" t="s">
         <v>464</v>
       </c>
       <c r="Q2" s="33" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="R2" s="6" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="S2" s="6" t="s">
         <v>444</v>
@@ -10071,19 +10074,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="6" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>13</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
@@ -10095,16 +10098,16 @@
       <c r="M3" s="6"/>
       <c r="N3" s="6"/>
       <c r="O3" s="6" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="P3" s="6" t="s">
         <v>464</v>
       </c>
       <c r="Q3" s="33" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="R3" s="6" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="S3" s="6" t="s">
         <v>444</v>
@@ -10114,19 +10117,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="6" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="29" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
@@ -10138,16 +10141,16 @@
       <c r="M4" s="6"/>
       <c r="N4" s="6"/>
       <c r="O4" s="6" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="P4" s="6" t="s">
         <v>464</v>
       </c>
       <c r="Q4" s="33" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="R4" s="6" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="S4" s="6" t="s">
         <v>444</v>
@@ -10157,19 +10160,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="6" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
@@ -10181,16 +10184,16 @@
       <c r="M5" s="6"/>
       <c r="N5" s="6"/>
       <c r="O5" s="6" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="P5" s="6" t="s">
         <v>464</v>
       </c>
       <c r="Q5" s="33" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="R5" s="6" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="S5" s="6" t="s">
         <v>444</v>
@@ -10200,17 +10203,17 @@
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="6" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="29" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
@@ -10222,16 +10225,16 @@
       <c r="M6" s="6"/>
       <c r="N6" s="6"/>
       <c r="O6" s="6" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="P6" s="6" t="s">
         <v>464</v>
       </c>
       <c r="Q6" s="33" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="R6" s="5" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="S6" s="6" t="s">
         <v>444</v>
@@ -10241,19 +10244,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="6" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="29" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
@@ -10265,16 +10268,16 @@
       <c r="M7" s="6"/>
       <c r="N7" s="6"/>
       <c r="O7" s="6" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="P7" s="6" t="s">
         <v>464</v>
       </c>
       <c r="Q7" s="33" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="R7" s="6" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="S7" s="6" t="s">
         <v>444</v>
@@ -10284,19 +10287,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="6" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="29" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
@@ -10308,16 +10311,16 @@
       <c r="M8" s="6"/>
       <c r="N8" s="6"/>
       <c r="O8" s="6" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="P8" s="6" t="s">
         <v>464</v>
       </c>
       <c r="Q8" s="33" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="R8" s="6" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="S8" s="6" t="s">
         <v>444</v>
@@ -10327,19 +10330,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="6" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="29" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
@@ -10351,16 +10354,16 @@
       <c r="M9" s="6"/>
       <c r="N9" s="6"/>
       <c r="O9" s="6" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="P9" s="6" t="s">
         <v>464</v>
       </c>
       <c r="Q9" s="33" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="R9" s="6" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="S9" s="6" t="s">
         <v>444</v>
@@ -10370,19 +10373,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="6" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>13</v>
       </c>
       <c r="D10" s="29" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
@@ -10394,16 +10397,16 @@
       <c r="M10" s="6"/>
       <c r="N10" s="6"/>
       <c r="O10" s="6" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="P10" s="6" t="s">
         <v>464</v>
       </c>
       <c r="Q10" s="33" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="R10" s="6" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="S10" s="6" t="s">
         <v>444</v>
@@ -10413,19 +10416,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="6" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>13</v>
       </c>
       <c r="D11" s="29" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
@@ -10437,16 +10440,16 @@
       <c r="M11" s="6"/>
       <c r="N11" s="6"/>
       <c r="O11" s="6" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="P11" s="6" t="s">
         <v>464</v>
       </c>
       <c r="Q11" s="33" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="R11" s="6" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="S11" s="6" t="s">
         <v>444</v>
@@ -10456,17 +10459,17 @@
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="6" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>13</v>
       </c>
       <c r="D12" s="34"/>
       <c r="E12" s="6" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
@@ -10478,16 +10481,16 @@
       <c r="M12" s="6"/>
       <c r="N12" s="6"/>
       <c r="O12" s="6" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="P12" s="6" t="s">
         <v>464</v>
       </c>
       <c r="Q12" s="33" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="R12" s="5" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="S12" s="6" t="s">
         <v>444</v>
@@ -10497,19 +10500,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="6" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>13</v>
       </c>
       <c r="D13" s="29" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
@@ -10521,16 +10524,16 @@
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
       <c r="O13" s="6" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="P13" s="6" t="s">
         <v>464</v>
       </c>
       <c r="Q13" s="33" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="R13" s="6" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="S13" s="6" t="s">
         <v>444</v>
@@ -10540,19 +10543,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="6" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>13</v>
       </c>
       <c r="D14" s="29" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
@@ -10564,16 +10567,16 @@
       <c r="M14" s="6"/>
       <c r="N14" s="6"/>
       <c r="O14" s="6" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="P14" s="6" t="s">
         <v>464</v>
       </c>
       <c r="Q14" s="33" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="R14" s="6" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="S14" s="6" t="s">
         <v>444</v>
@@ -10583,19 +10586,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="6" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>13</v>
       </c>
       <c r="D15" s="29" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
@@ -10607,16 +10610,16 @@
       <c r="M15" s="6"/>
       <c r="N15" s="6"/>
       <c r="O15" s="6" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="P15" s="6" t="s">
         <v>464</v>
       </c>
       <c r="Q15" s="33" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="R15" s="6" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="S15" s="6" t="s">
         <v>444</v>
@@ -10626,19 +10629,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="6" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>13</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
@@ -10650,16 +10653,16 @@
       <c r="M16" s="6"/>
       <c r="N16" s="6"/>
       <c r="O16" s="6" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="P16" s="6" t="s">
         <v>464</v>
       </c>
       <c r="Q16" s="33" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="R16" s="6" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="S16" s="6" t="s">
         <v>444</v>
@@ -10669,17 +10672,17 @@
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="6" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="29" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
@@ -10691,16 +10694,16 @@
       <c r="M17" s="6"/>
       <c r="N17" s="6"/>
       <c r="O17" s="6" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="P17" s="6" t="s">
         <v>464</v>
       </c>
       <c r="Q17" s="33" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="R17" s="6" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="S17" s="6" t="s">
         <v>444</v>
@@ -10710,19 +10713,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="6" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="D18" s="29" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
@@ -10734,16 +10737,16 @@
       <c r="M18" s="6"/>
       <c r="N18" s="6"/>
       <c r="O18" s="6" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="P18" s="6" t="s">
         <v>464</v>
       </c>
       <c r="Q18" s="33" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="R18" s="6" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="S18" s="6" t="s">
         <v>444</v>
@@ -10753,19 +10756,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="6" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="D19" s="29" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
@@ -10777,16 +10780,16 @@
       <c r="M19" s="6"/>
       <c r="N19" s="6"/>
       <c r="O19" s="6" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="P19" s="6" t="s">
         <v>464</v>
       </c>
       <c r="Q19" s="33" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="R19" s="6" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="S19" s="6" t="s">
         <v>444</v>
@@ -10796,19 +10799,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="6" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="D20" s="29" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
@@ -10820,16 +10823,16 @@
       <c r="M20" s="6"/>
       <c r="N20" s="6"/>
       <c r="O20" s="6" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="P20" s="6" t="s">
         <v>464</v>
       </c>
       <c r="Q20" s="33" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="R20" s="6" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="S20" s="6" t="s">
         <v>444</v>
@@ -10839,19 +10842,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="6" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="D21" s="29" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
@@ -10863,16 +10866,16 @@
       <c r="M21" s="6"/>
       <c r="N21" s="6"/>
       <c r="O21" s="6" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="P21" s="6" t="s">
         <v>464</v>
       </c>
       <c r="Q21" s="33" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="R21" s="6" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="S21" s="6" t="s">
         <v>444</v>
@@ -10882,19 +10885,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="6" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="D22" s="29" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
@@ -10906,16 +10909,16 @@
       <c r="M22" s="6"/>
       <c r="N22" s="6"/>
       <c r="O22" s="6" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="P22" s="6" t="s">
         <v>464</v>
       </c>
       <c r="Q22" s="33" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="R22" s="6" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="S22" s="6" t="s">
         <v>444</v>
@@ -10925,19 +10928,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="6" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="D23" s="29" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
@@ -10949,16 +10952,16 @@
       <c r="M23" s="6"/>
       <c r="N23" s="6"/>
       <c r="O23" s="6" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="P23" s="6" t="s">
         <v>464</v>
       </c>
       <c r="Q23" s="33" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="R23" s="6" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="S23" s="6" t="s">
         <v>444</v>
@@ -10968,16 +10971,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="6" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>13</v>
       </c>
       <c r="D24" s="29" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
@@ -10990,16 +10993,16 @@
       <c r="M24" s="6"/>
       <c r="N24" s="6"/>
       <c r="O24" s="6" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="P24" s="6" t="s">
         <v>464</v>
       </c>
       <c r="Q24" s="33" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="R24" s="6" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="S24" s="6" t="s">
         <v>444</v>
@@ -11009,19 +11012,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="6" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>13</v>
       </c>
       <c r="D25" s="29" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
@@ -11033,16 +11036,16 @@
       <c r="M25" s="6"/>
       <c r="N25" s="6"/>
       <c r="O25" s="6" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="P25" s="6" t="s">
         <v>464</v>
       </c>
       <c r="Q25" s="33" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="R25" s="6" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="S25" s="6" t="s">
         <v>444</v>
@@ -11052,22 +11055,22 @@
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="6" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>13</v>
       </c>
       <c r="D26" s="29" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
@@ -11078,16 +11081,16 @@
       <c r="M26" s="6"/>
       <c r="N26" s="6"/>
       <c r="O26" s="6" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="P26" s="6" t="s">
         <v>464</v>
       </c>
       <c r="Q26" s="33" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="R26" s="6" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="S26" s="6" t="s">
         <v>444</v>
@@ -11097,19 +11100,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
       <c r="A27" s="6" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>13</v>
       </c>
       <c r="D27" s="29" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
@@ -11121,85 +11124,85 @@
       <c r="M27" s="6"/>
       <c r="N27" s="6"/>
       <c r="O27" s="6" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="P27" s="6" t="s">
         <v>464</v>
       </c>
       <c r="Q27" s="33" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="R27" s="6" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="S27" s="6" t="s">
         <v>442</v>
       </c>
       <c r="T27" s="6" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="U27" s="24"/>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
       <c r="A28" s="6" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>12</v>
       </c>
       <c r="D28" s="29" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="J28" s="6" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="K28" s="6" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="L28" s="6" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="M28" s="6" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="N28" s="6" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="O28" s="6" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="P28" s="6" t="s">
         <v>464</v>
       </c>
       <c r="Q28" s="33" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="R28" s="6" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="S28" s="6" t="s">
         <v>442</v>
       </c>
       <c r="T28" s="6" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="U28" s="24"/>
     </row>
@@ -11244,7 +11247,7 @@
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="29" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>459</v>
@@ -11279,19 +11282,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="29" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>464</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>442</v>
@@ -11315,16 +11318,16 @@
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="29"/>
       <c r="B3" s="6" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>464</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>442</v>
@@ -11347,19 +11350,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="29" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>464</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>442</v>
@@ -11382,19 +11385,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="29" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>464</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>444</v>
@@ -11417,19 +11420,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="29" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>464</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>442</v>
@@ -11452,19 +11455,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="29" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>464</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>442</v>
@@ -11490,16 +11493,16 @@
         <v>1000000</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>464</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>444</v>
@@ -11522,19 +11525,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="29" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>464</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>444</v>
@@ -11567,7 +11570,7 @@
   </sheetPr>
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -11591,10 +11594,10 @@
         <v>29</v>
       </c>
       <c r="C1" s="29" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>459</v>
@@ -11622,19 +11625,19 @@
       </c>
       <c r="C2" s="29"/>
       <c r="D2" s="6" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>464</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>444</v>
@@ -11652,19 +11655,19 @@
         <v>123</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>464</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="I3" s="6" t="s">
         <v>444</v>
@@ -11679,22 +11682,22 @@
         <v>34</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>464</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>444</v>
@@ -11715,16 +11718,16 @@
         <v>34</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>464</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="I5" s="6" t="s">
         <v>444</v>
@@ -11743,16 +11746,16 @@
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="5" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>464</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="I6" s="6" t="s">
         <v>444</v>
@@ -11770,19 +11773,19 @@
         <v>34</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>464</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="I7" s="6" t="s">
         <v>444</v>
@@ -11800,19 +11803,19 @@
         <v>34</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>464</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="I8" s="6" t="s">
         <v>442</v>
@@ -11851,10 +11854,10 @@
         <v>28</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>459</v>
@@ -11872,28 +11875,28 @@
         <v>440</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="6"/>
       <c r="B2" s="6" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>464</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>444</v>
@@ -11902,25 +11905,25 @@
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="6" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>464</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>444</v>
@@ -11929,25 +11932,25 @@
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="6" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>464</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="H4" s="6" t="s">
         <v>444</v>
@@ -11956,25 +11959,25 @@
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="6" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>464</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="H5" s="6" t="s">
         <v>444</v>
@@ -11983,25 +11986,25 @@
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="6" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>464</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="H6" s="6" t="s">
         <v>444</v>
@@ -12010,25 +12013,25 @@
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="6" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>464</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="H7" s="6" t="s">
         <v>444</v>
@@ -12037,25 +12040,25 @@
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="6" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>464</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="H8" s="6" t="s">
         <v>444</v>
@@ -12068,19 +12071,19 @@
       </c>
       <c r="B9" s="29"/>
       <c r="C9" s="6" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>464</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="H9" s="6" t="s">
         <v>444</v>
@@ -12092,22 +12095,22 @@
         <v>1</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>464</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="H10" s="6" t="s">
         <v>444</v>
@@ -12119,22 +12122,22 @@
         <v>1</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>464</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="H11" s="6" t="s">
         <v>444</v>
@@ -12146,20 +12149,20 @@
         <v>1</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="C12" s="29"/>
       <c r="D12" s="5" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>464</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="H12" s="6" t="s">
         <v>444</v>
@@ -12171,22 +12174,22 @@
         <v>1</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>464</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="H13" s="6" t="s">
         <v>444</v>
@@ -12198,28 +12201,28 @@
         <v>1</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>464</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="H14" s="6" t="s">
         <v>444</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
@@ -12227,28 +12230,28 @@
         <v>1</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>464</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="H15" s="6" t="s">
         <v>444</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
@@ -12256,28 +12259,28 @@
         <v>1</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>464</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="H16" s="6" t="s">
         <v>442</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
     </row>
   </sheetData>
@@ -12318,31 +12321,31 @@
         <v>27</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="K1" s="6" t="s">
         <v>459</v>
@@ -12363,7 +12366,7 @@
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="6"/>
       <c r="B2" s="6" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
@@ -12374,16 +12377,16 @@
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
       <c r="K2" s="6" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="L2" s="6" t="s">
         <v>464</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="O2" s="6" t="s">
         <v>444</v>
@@ -12391,10 +12394,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="6" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
@@ -12405,16 +12408,16 @@
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
       <c r="K3" s="6" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="L3" s="6" t="s">
         <v>464</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="O3" s="6" t="s">
         <v>444</v>
@@ -12422,7 +12425,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="6" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -12434,16 +12437,16 @@
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
       <c r="K4" s="6" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="L4" s="6" t="s">
         <v>464</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="O4" s="6" t="s">
         <v>444</v>
@@ -12451,10 +12454,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="6" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
@@ -12465,16 +12468,16 @@
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
       <c r="K5" s="6" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="L5" s="6" t="s">
         <v>464</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="O5" s="6" t="s">
         <v>444</v>
@@ -12482,10 +12485,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="6" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
@@ -12496,16 +12499,16 @@
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
       <c r="K6" s="6" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="L6" s="6" t="s">
         <v>464</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="O6" s="6" t="s">
         <v>442</v>
@@ -12513,46 +12516,46 @@
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="6" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="D7" s="6" t="s">
+        <v>520</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>521</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>522</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>523</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>524</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>525</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>526</v>
+      </c>
+      <c r="K7" s="6" t="s">
         <v>519</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>520</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>521</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>522</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>523</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>524</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>525</v>
-      </c>
-      <c r="K7" s="6" t="s">
-        <v>518</v>
       </c>
       <c r="L7" s="6" t="s">
         <v>464</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="O7" s="6" t="s">
         <v>442</v>
@@ -12604,7 +12607,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="6" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>464</v>
@@ -12613,7 +12616,7 @@
         <v>465</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>444</v>
@@ -12624,7 +12627,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="6" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>464</v>
@@ -12633,7 +12636,7 @@
         <v>465</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>444</v>
@@ -12644,16 +12647,16 @@
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="6" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>464</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>442</v>
@@ -12748,7 +12751,9 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
-      <c r="A3" s="7"/>
+      <c r="A3" s="7" t="s">
+        <v>483</v>
+      </c>
       <c r="B3" s="31">
         <v>3</v>
       </c>
@@ -12765,7 +12770,7 @@
         <v>465</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>29</v>
@@ -12776,7 +12781,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="6" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="B4" s="31">
         <v>5</v>
@@ -12794,7 +12799,7 @@
         <v>465</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="H4" s="6" t="s">
         <v>29</v>

</xml_diff>